<commit_message>
Image & Logo upload
</commit_message>
<xml_diff>
--- a/scripts/data_v2_results.xlsx
+++ b/scripts/data_v2_results.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -428,6 +428,9 @@
       <c r="O1" t="str">
         <v>longitude</v>
       </c>
+      <c r="P1" t="str">
+        <v>position</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -516,10 +519,10 @@
         <v>Entreprise</v>
       </c>
       <c r="N3">
-        <v>50.619205</v>
+        <v>50.608265</v>
       </c>
       <c r="O3">
-        <v>3.143694</v>
+        <v>3.16046</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
@@ -698,14 +701,14 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -759,6 +762,9 @@
       <c r="P1" t="str">
         <v>longitude</v>
       </c>
+      <c r="Q1" t="str">
+        <v>position</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -854,10 +860,10 @@
         <v>Labo</v>
       </c>
       <c r="O3">
-        <v>50.513812</v>
+        <v>50.518746</v>
       </c>
       <c r="P3">
-        <v>2.658348</v>
+        <v>2.645622</v>
       </c>
     </row>
     <row r="4">
@@ -909,14 +915,14 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -982,6 +988,9 @@
       <c r="T1" t="str">
         <v>longitude</v>
       </c>
+      <c r="U1" t="str">
+        <v>position</v>
+      </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
@@ -1157,15 +1166,15 @@
         <v>Formation</v>
       </c>
       <c r="S4">
-        <v>50.93243</v>
+        <v>50.934099</v>
       </c>
       <c r="T4">
-        <v>1.820529</v>
+        <v>1.808739</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:U4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>